<commit_message>
Stats model ready, KNN and Scikit model on the way
</commit_message>
<xml_diff>
--- a/Data2/Birthweight_explored.xlsx
+++ b/Data2/Birthweight_explored.xlsx
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>-1</v>
@@ -901,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC4">
         <v>-1</v>
@@ -1106,16 +1106,16 @@
         <v>24</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <v>-1</v>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="AA7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>-1</v>
       </c>
       <c r="AD7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE7">
         <v>-1</v>
@@ -1320,7 +1320,7 @@
         <v>24</v>
       </c>
       <c r="Y8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>0</v>
       </c>
       <c r="AA9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>-1</v>
@@ -1855,7 +1855,7 @@
         <v>32</v>
       </c>
       <c r="Y13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -2075,10 +2075,10 @@
         <v>0</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC15">
         <v>-1</v>
@@ -2283,7 +2283,7 @@
         <v>33</v>
       </c>
       <c r="Y17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="AB18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>-1</v>
@@ -2497,7 +2497,7 @@
         <v>32</v>
       </c>
       <c r="Y19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -2604,7 +2604,7 @@
         <v>30</v>
       </c>
       <c r="Y20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z20">
         <v>0</v>
@@ -2925,7 +2925,7 @@
         <v>28</v>
       </c>
       <c r="Y23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -3032,7 +3032,7 @@
         <v>32</v>
       </c>
       <c r="Y24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -3139,7 +3139,7 @@
         <v>24</v>
       </c>
       <c r="Y25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z25">
         <v>0</v>
@@ -3246,7 +3246,7 @@
         <v>30</v>
       </c>
       <c r="Y26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26">
         <v>0</v>
@@ -3674,7 +3674,7 @@
         <v>24</v>
       </c>
       <c r="Y30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z30">
         <v>0</v>
@@ -3888,7 +3888,7 @@
         <v>32</v>
       </c>
       <c r="Y32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>-1</v>
       </c>
       <c r="AD34">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE34">
         <v>0</v>
@@ -4851,7 +4851,7 @@
         <v>23</v>
       </c>
       <c r="Y41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z41">
         <v>0</v>
@@ -5065,7 +5065,7 @@
         <v>32</v>
       </c>
       <c r="Y43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z43">
         <v>0</v>
@@ -5279,7 +5279,7 @@
         <v>23</v>
       </c>
       <c r="Y45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z45">
         <v>0</v>
@@ -5386,7 +5386,7 @@
         <v>22</v>
       </c>
       <c r="Y46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z46">
         <v>-1</v>
@@ -5508,7 +5508,7 @@
         <v>0</v>
       </c>
       <c r="AD47">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE47">
         <v>0</v>
@@ -5600,7 +5600,7 @@
         <v>24</v>
       </c>
       <c r="Y48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z48">
         <v>0</v>
@@ -5609,7 +5609,7 @@
         <v>0</v>
       </c>
       <c r="AB48">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC48">
         <v>-1</v>
@@ -5707,7 +5707,7 @@
         <v>24</v>
       </c>
       <c r="Y49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z49">
         <v>0</v>
@@ -5814,7 +5814,7 @@
         <v>28</v>
       </c>
       <c r="Y50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z50">
         <v>0</v>
@@ -5921,7 +5921,7 @@
         <v>31</v>
       </c>
       <c r="Y51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z51">
         <v>0</v>
@@ -6670,7 +6670,7 @@
         <v>24</v>
       </c>
       <c r="Y58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z58">
         <v>0</v>
@@ -6679,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="AB58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC58">
         <v>-1</v>
@@ -6884,7 +6884,7 @@
         <v>30</v>
       </c>
       <c r="Y60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z60">
         <v>0</v>
@@ -7098,7 +7098,7 @@
         <v>26</v>
       </c>
       <c r="Y62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z62">
         <v>0</v>
@@ -7205,7 +7205,7 @@
         <v>26</v>
       </c>
       <c r="Y63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z63">
         <v>0</v>
@@ -7419,7 +7419,7 @@
         <v>26</v>
       </c>
       <c r="Y65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z65">
         <v>0</v>
@@ -7639,7 +7639,7 @@
         <v>0</v>
       </c>
       <c r="AA67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB67">
         <v>-1</v>
@@ -7847,7 +7847,7 @@
         <v>28</v>
       </c>
       <c r="Y69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z69">
         <v>0</v>
@@ -8168,7 +8168,7 @@
         <v>28</v>
       </c>
       <c r="Y72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z72">
         <v>0</v>
@@ -8275,7 +8275,7 @@
         <v>33</v>
       </c>
       <c r="Y73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z73">
         <v>0</v>
@@ -8382,7 +8382,7 @@
         <v>24</v>
       </c>
       <c r="Y74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z74">
         <v>0</v>
@@ -8489,7 +8489,7 @@
         <v>32</v>
       </c>
       <c r="Y75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z75">
         <v>0</v>
@@ -8596,7 +8596,7 @@
         <v>27</v>
       </c>
       <c r="Y76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z76">
         <v>0</v>
@@ -9024,7 +9024,7 @@
         <v>34</v>
       </c>
       <c r="Y80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z80">
         <v>0</v>
@@ -9238,7 +9238,7 @@
         <v>32</v>
       </c>
       <c r="Y82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z82">
         <v>0</v>
@@ -9458,7 +9458,7 @@
         <v>0</v>
       </c>
       <c r="AA84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB84">
         <v>0</v>
@@ -9773,7 +9773,7 @@
         <v>23</v>
       </c>
       <c r="Y87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z87">
         <v>0</v>
@@ -9996,7 +9996,7 @@
         <v>0</v>
       </c>
       <c r="AB89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC89">
         <v>-1</v>
@@ -10201,7 +10201,7 @@
         <v>26</v>
       </c>
       <c r="Y91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z91">
         <v>0</v>
@@ -10308,7 +10308,7 @@
         <v>25</v>
       </c>
       <c r="Y92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z92">
         <v>0</v>
@@ -10629,7 +10629,7 @@
         <v>24</v>
       </c>
       <c r="Y95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z95">
         <v>0</v>
@@ -11066,7 +11066,7 @@
         <v>0</v>
       </c>
       <c r="AB99">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC99">
         <v>-1</v>
@@ -11164,7 +11164,7 @@
         <v>24</v>
       </c>
       <c r="Y100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z100">
         <v>0</v>
@@ -11271,13 +11271,13 @@
         <v>31</v>
       </c>
       <c r="Y101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z101">
         <v>0</v>
       </c>
       <c r="AA101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB101">
         <v>0</v>
@@ -11378,7 +11378,7 @@
         <v>32</v>
       </c>
       <c r="Y102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z102">
         <v>0</v>
@@ -11592,7 +11592,7 @@
         <v>33</v>
       </c>
       <c r="Y104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z104">
         <v>0</v>
@@ -11699,7 +11699,7 @@
         <v>31</v>
       </c>
       <c r="Y105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z105">
         <v>0</v>
@@ -11806,7 +11806,7 @@
         <v>33</v>
       </c>
       <c r="Y106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z106">
         <v>0</v>
@@ -11913,7 +11913,7 @@
         <v>32</v>
       </c>
       <c r="Y107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z107">
         <v>0</v>
@@ -12356,7 +12356,7 @@
         <v>-1</v>
       </c>
       <c r="AD111">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE111">
         <v>0</v>
@@ -12448,13 +12448,13 @@
         <v>23</v>
       </c>
       <c r="Y112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z112">
         <v>0</v>
       </c>
       <c r="AA112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB112">
         <v>0</v>
@@ -12778,7 +12778,7 @@
         <v>0</v>
       </c>
       <c r="AB115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC115">
         <v>-1</v>
@@ -12876,7 +12876,7 @@
         <v>28</v>
       </c>
       <c r="Y116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z116">
         <v>0</v>
@@ -12983,7 +12983,7 @@
         <v>30</v>
       </c>
       <c r="Y117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z117">
         <v>0</v>
@@ -12992,7 +12992,7 @@
         <v>0</v>
       </c>
       <c r="AB117">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC117">
         <v>-1</v>
@@ -13310,7 +13310,7 @@
         <v>0</v>
       </c>
       <c r="AA120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB120">
         <v>0</v>
@@ -13411,7 +13411,7 @@
         <v>23</v>
       </c>
       <c r="Y121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z121">
         <v>0</v>
@@ -13625,7 +13625,7 @@
         <v>27</v>
       </c>
       <c r="Y123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z123">
         <v>0</v>
@@ -13732,7 +13732,7 @@
         <v>33</v>
       </c>
       <c r="Y124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z124">
         <v>0</v>
@@ -13741,7 +13741,7 @@
         <v>0</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
         <v>-1</v>
@@ -14053,7 +14053,7 @@
         <v>33</v>
       </c>
       <c r="Y127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z127">
         <v>0</v>
@@ -14160,22 +14160,22 @@
         <v>16</v>
       </c>
       <c r="Y128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z128">
         <v>-1</v>
       </c>
       <c r="AA128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB128">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC128">
         <v>-1</v>
       </c>
       <c r="AD128">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE128">
         <v>-1</v>
@@ -14267,7 +14267,7 @@
         <v>24</v>
       </c>
       <c r="Y129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z129">
         <v>0</v>
@@ -14374,7 +14374,7 @@
         <v>24</v>
       </c>
       <c r="Y130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z130">
         <v>0</v>
@@ -14487,7 +14487,7 @@
         <v>0</v>
       </c>
       <c r="AA131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB131">
         <v>0</v>
@@ -14802,7 +14802,7 @@
         <v>28</v>
       </c>
       <c r="Y134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z134">
         <v>0</v>
@@ -15016,7 +15016,7 @@
         <v>30</v>
       </c>
       <c r="Y136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z136">
         <v>0</v>
@@ -15236,10 +15236,10 @@
         <v>0</v>
       </c>
       <c r="AA138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB138">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC138">
         <v>-1</v>
@@ -15346,7 +15346,7 @@
         <v>0</v>
       </c>
       <c r="AB139">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC139">
         <v>-1</v>
@@ -15979,7 +15979,7 @@
         <v>29</v>
       </c>
       <c r="Y145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z145">
         <v>0</v>
@@ -15988,7 +15988,7 @@
         <v>0</v>
       </c>
       <c r="AB145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC145">
         <v>-1</v>
@@ -16199,10 +16199,10 @@
         <v>0</v>
       </c>
       <c r="AA147">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB147">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC147">
         <v>-1</v>
@@ -16514,7 +16514,7 @@
         <v>24</v>
       </c>
       <c r="Y150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z150">
         <v>0</v>
@@ -16529,7 +16529,7 @@
         <v>-1</v>
       </c>
       <c r="AD150">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE150">
         <v>0</v>
@@ -16621,7 +16621,7 @@
         <v>33</v>
       </c>
       <c r="Y151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z151">
         <v>0</v>
@@ -16942,7 +16942,7 @@
         <v>24</v>
       </c>
       <c r="Y154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z154">
         <v>0</v>
@@ -17272,7 +17272,7 @@
         <v>0</v>
       </c>
       <c r="AB157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC157">
         <v>-1</v>
@@ -17593,7 +17593,7 @@
         <v>0</v>
       </c>
       <c r="AB160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC160">
         <v>-1</v>
@@ -17691,7 +17691,7 @@
         <v>24</v>
       </c>
       <c r="Y161">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z161">
         <v>0</v>
@@ -17905,7 +17905,7 @@
         <v>24</v>
       </c>
       <c r="Y163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z163">
         <v>0</v>
@@ -18119,7 +18119,7 @@
         <v>24</v>
       </c>
       <c r="Y165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z165">
         <v>0</v>
@@ -18235,7 +18235,7 @@
         <v>0</v>
       </c>
       <c r="AB166">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC166">
         <v>-1</v>
@@ -18339,7 +18339,7 @@
         <v>0</v>
       </c>
       <c r="AA167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB167">
         <v>-1</v>
@@ -18547,7 +18547,7 @@
         <v>28</v>
       </c>
       <c r="Y169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z169">
         <v>0</v>
@@ -18761,7 +18761,7 @@
         <v>32</v>
       </c>
       <c r="Y171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z171">
         <v>0</v>
@@ -18981,7 +18981,7 @@
         <v>0</v>
       </c>
       <c r="AA173">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB173">
         <v>0</v>
@@ -19082,7 +19082,7 @@
         <v>30</v>
       </c>
       <c r="Y174">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z174">
         <v>0</v>
@@ -19189,7 +19189,7 @@
         <v>25</v>
       </c>
       <c r="Y175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z175">
         <v>0</v>
@@ -19724,7 +19724,7 @@
         <v>32</v>
       </c>
       <c r="Y180">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z180">
         <v>0</v>
@@ -20152,7 +20152,7 @@
         <v>31</v>
       </c>
       <c r="Y184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z184">
         <v>0</v>
@@ -20259,7 +20259,7 @@
         <v>28</v>
       </c>
       <c r="Y185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z185">
         <v>0</v>
@@ -20372,7 +20372,7 @@
         <v>0</v>
       </c>
       <c r="AA186">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB186">
         <v>0</v>
@@ -20580,7 +20580,7 @@
         <v>32</v>
       </c>
       <c r="Y188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z188">
         <v>0</v>
@@ -20901,7 +20901,7 @@
         <v>27</v>
       </c>
       <c r="Y191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z191">
         <v>0</v>
@@ -21008,13 +21008,13 @@
         <v>27</v>
       </c>
       <c r="Y192">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z192">
         <v>0</v>
       </c>
       <c r="AA192">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB192">
         <v>0</v>
@@ -21121,7 +21121,7 @@
         <v>0</v>
       </c>
       <c r="AA193">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB193">
         <v>0</v>
@@ -21222,7 +21222,7 @@
         <v>30</v>
       </c>
       <c r="Y194">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z194">
         <v>0</v>
@@ -21445,7 +21445,7 @@
         <v>0</v>
       </c>
       <c r="AB196">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC196">
         <v>-1</v>

</xml_diff>